<commit_message>
hitori: change flag, gotta be a little bit more obscure
</commit_message>
<xml_diff>
--- a/hitori/docs/题目基本信息.xlsx
+++ b/hitori/docs/题目基本信息.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\src\github.com\Riatre\aliyunctf-2022-challenges\hitori\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD83717-053E-4815-AC6B-DA07CB786DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8150271B-5342-4CF8-9503-F5985770075E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,21 +58,17 @@
   </si>
   <si>
     <t>pwn-hitori</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Tired of having to reverse engineer the binary before you can actually start on finding bugs and writing exploits? Don't want to write tedious scripts just to be able to talk to the service? We heard! Check out our source-available text-based menu challenge. Draw something, enjoy cool filters and maybe even a shell!
 nc &lt;ip&gt; 1337</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>你是否也因为做 Pwn 题开始挖洞和写利用之前还得花时间逆向而累觉不爱？是否再也不想写莫名其妙的交互脚本只为了能触发服务里的正常功能？我们听到了你的声音！快来试试我们这个提供源码、纯文本交互的菜单题吧。画点好康的，加点酷炫滤镜，顺便看看能不能拿个 shell！
 nc &lt;ip&gt; 1337</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>aliyunctf{smashi_your_SUIbscribe_button_now_do_it_quickly_pleaSEI_visit_this_channel_UC5CwaMl1eIgY8h02uZw7u8A}</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -105,7 +101,7 @@
       </rPr>
       <t>的中文信息</t>
     </r>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -128,18 +124,28 @@
       </rPr>
       <t xml:space="preserve"> health check</t>
     </r>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>aliyunctf{smashi_your_SUIbscribe_button_now_do_it_quickly_pleaSEI_UC5CwaMl1eIgY8h02uZw7u8A}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -207,12 +213,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -431,7 +437,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -481,7 +487,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
@@ -493,7 +499,7 @@
         <v>1337</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -504,7 +510,7 @@
         <v>12</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1505,7 +1511,7 @@
     <row r="999" ht="13.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1000" ht="13.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>